<commit_message>
Adding support for dairy and phosphorus in progress table spreadsheet.
</commit_message>
<xml_diff>
--- a/test/progress_table.xlsx
+++ b/test/progress_table.xlsx
@@ -174,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>progress towards targets indicators</t>
   </si>
@@ -237,12 +237,6 @@
 average sediment
 load between 2009
 And 2011.</t>
-  </si>
-  <si>
-    <t>Reduction in annual
-averages pesticide
-load between 2009
-and 2011</t>
   </si>
   <si>
     <t>Target: 50 per cent
@@ -342,12 +336,33 @@
   <si>
     <t>very poor</t>
   </si>
+  <si>
+    <t>Dairy</t>
+  </si>
+  <si>
+    <t>Proportion of dairy farmers who adopted improved  practices between 2009 and 2011.</t>
+  </si>
+  <si>
+    <t>Target: 50 per cent by 2013</t>
+  </si>
+  <si>
+    <t>Phosphorus</t>
+  </si>
+  <si>
+    <t>Reduction in annual average total phosphorus load between 2009 and 2011.</t>
+  </si>
+  <si>
+    <t>Reduction in annual
+averages pesticide
+load between 2009
+and 2011.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -374,8 +389,14 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -452,6 +473,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
         <bgColor rgb="FF008080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -464,10 +503,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -491,9 +531,14 @@
     <xf numFmtId="9" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -844,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -863,7 +908,7 @@
     <col min="10" max="1025" width="11.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -888,8 +933,14 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="57.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="57.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
@@ -909,38 +960,50 @@
         <v>13</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="C4" s="3">
         <v>0.17</v>
@@ -963,13 +1026,19 @@
       <c r="I4" s="13">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="46.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J4" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="K4" s="22">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="46.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="C5" s="12">
         <v>0.33</v>
@@ -986,13 +1055,16 @@
         <v>0.06</v>
       </c>
       <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" ht="68.650000000000006" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K5" s="24">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="68.650000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C6" s="3">
         <v>0.16</v>
@@ -1015,13 +1087,16 @@
       <c r="I6" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K6" s="23">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C7" s="13">
         <v>0.2</v>
@@ -1044,13 +1119,16 @@
       <c r="I7" s="13">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="57.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K7" s="22">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="57.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="C8" s="12">
         <v>0.36</v>
@@ -1073,13 +1151,16 @@
       <c r="I8" s="12">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="68.650000000000006" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K8" s="22">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="68.650000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="C9" s="17">
         <v>0.16</v>
@@ -1102,13 +1183,16 @@
       <c r="I9" s="3">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="57.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K9" s="21">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="57.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="C10" s="3">
         <v>0.13</v>
@@ -1130,6 +1214,9 @@
       </c>
       <c r="I10" s="6">
         <v>0.17</v>
+      </c>
+      <c r="K10" s="21">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -1159,27 +1246,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding tests for detector.
</commit_message>
<xml_diff>
--- a/test/progress_table.xlsx
+++ b/test/progress_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,9 +13,13 @@
   </bookViews>
   <sheets>
     <sheet name="progress" sheetId="1" r:id="rId1"/>
-    <sheet name="condition" sheetId="2" r:id="rId2"/>
+    <sheet name="imported values" sheetId="3" r:id="rId2"/>
+    <sheet name="condition" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -173,8 +177,42 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Tim Dettrick</author>
+  </authors>
+  <commentList>
+    <comment ref="A4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tim Dettrick:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Should be detected as Very Good.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>progress towards targets indicators</t>
   </si>
@@ -624,6 +662,50 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="avgCover_ordered"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="23">
+          <cell r="AA23">
+            <v>74.8</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="AA24">
+            <v>78.2</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="AA25">
+            <v>88.1</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="AA26">
+            <v>85</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="AA27">
+            <v>88.3</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="AA28">
+            <v>77.7</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -891,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1014,8 +1096,9 @@
       <c r="E4" s="3">
         <v>0.25</v>
       </c>
-      <c r="F4" s="14">
-        <v>0.91</v>
+      <c r="F4" s="21">
+        <f>'imported values'!A2/100</f>
+        <v>0.77700000000000002</v>
       </c>
       <c r="G4" s="3">
         <v>7.0000000000000007E-2</v>
@@ -1076,7 +1159,8 @@
         <v>0.24</v>
       </c>
       <c r="F6" s="19">
-        <v>0.95</v>
+        <f>'imported values'!A4/100</f>
+        <v>0.88300000000000001</v>
       </c>
       <c r="G6" s="16">
         <v>0.04</v>
@@ -1108,7 +1192,8 @@
         <v>0.27</v>
       </c>
       <c r="F7" s="14">
-        <v>0.92</v>
+        <f>'imported values'!A5/100</f>
+        <v>0.748</v>
       </c>
       <c r="G7" s="5">
         <v>0.08</v>
@@ -1140,7 +1225,8 @@
         <v>0.47</v>
       </c>
       <c r="F8" s="14">
-        <v>0.92</v>
+        <f>'imported values'!A6/100</f>
+        <v>0.88099999999999989</v>
       </c>
       <c r="G8" s="13">
         <v>0.13</v>
@@ -1172,7 +1258,8 @@
         <v>0.13</v>
       </c>
       <c r="F9" s="14">
-        <v>0.9</v>
+        <f>'imported values'!A7/100</f>
+        <v>0.78200000000000003</v>
       </c>
       <c r="G9" s="5">
         <v>0.02</v>
@@ -1204,7 +1291,8 @@
         <v>0.25</v>
       </c>
       <c r="F10" s="14">
-        <v>0.93</v>
+        <f>'imported values'!A8/100</f>
+        <v>0.85</v>
       </c>
       <c r="G10" s="3">
         <v>0.08</v>
@@ -1221,16 +1309,76 @@
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="21">
+        <f>[1]avgCover_ordered!$AA$28</f>
+        <v>77.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="19">
+        <f>[1]avgCover_ordered!$AA$27</f>
+        <v>88.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="14">
+        <f>[1]avgCover_ordered!$AA$23</f>
+        <v>74.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
+        <f>[1]avgCover_ordered!$AA$25</f>
+        <v>88.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="14">
+        <f>[1]avgCover_ordered!$AA$24</f>
+        <v>78.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="14">
+        <f>[1]avgCover_ordered!$AA$26</f>
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Correcting the external references to point to the right cells.
</commit_message>
<xml_diff>
--- a/test/progress_table.xlsx
+++ b/test/progress_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="257"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="257" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="progress" sheetId="1" r:id="rId1"/>
@@ -673,33 +673,33 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="23">
-          <cell r="AA23">
-            <v>74.8</v>
+          <cell r="Z23">
+            <v>91.7</v>
           </cell>
         </row>
         <row r="24">
-          <cell r="AA24">
-            <v>78.2</v>
+          <cell r="Z24">
+            <v>90.2</v>
           </cell>
         </row>
         <row r="25">
-          <cell r="AA25">
-            <v>88.1</v>
+          <cell r="Z25">
+            <v>92.4</v>
           </cell>
         </row>
         <row r="26">
-          <cell r="AA26">
-            <v>85</v>
+          <cell r="Z26">
+            <v>93.1</v>
           </cell>
         </row>
         <row r="27">
-          <cell r="AA27">
-            <v>88.3</v>
+          <cell r="Z27">
+            <v>94.7</v>
           </cell>
         </row>
         <row r="28">
-          <cell r="AA28">
-            <v>77.7</v>
+          <cell r="Z28">
+            <v>91.2</v>
           </cell>
         </row>
       </sheetData>
@@ -973,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1098,7 +1098,7 @@
       </c>
       <c r="F4" s="21">
         <f>'imported values'!A2/100</f>
-        <v>0.77700000000000002</v>
+        <v>0.91200000000000003</v>
       </c>
       <c r="G4" s="3">
         <v>7.0000000000000007E-2</v>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="F6" s="19">
         <f>'imported values'!A4/100</f>
-        <v>0.88300000000000001</v>
+        <v>0.94700000000000006</v>
       </c>
       <c r="G6" s="16">
         <v>0.04</v>
@@ -1193,7 +1193,7 @@
       </c>
       <c r="F7" s="14">
         <f>'imported values'!A5/100</f>
-        <v>0.748</v>
+        <v>0.91700000000000004</v>
       </c>
       <c r="G7" s="5">
         <v>0.08</v>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="F8" s="14">
         <f>'imported values'!A6/100</f>
-        <v>0.88099999999999989</v>
+        <v>0.92400000000000004</v>
       </c>
       <c r="G8" s="13">
         <v>0.13</v>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="F9" s="14">
         <f>'imported values'!A7/100</f>
-        <v>0.78200000000000003</v>
+        <v>0.90200000000000002</v>
       </c>
       <c r="G9" s="5">
         <v>0.02</v>
@@ -1292,7 +1292,7 @@
       </c>
       <c r="F10" s="14">
         <f>'imported values'!A8/100</f>
-        <v>0.85</v>
+        <v>0.93099999999999994</v>
       </c>
       <c r="G10" s="3">
         <v>0.08</v>
@@ -1322,8 +1322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1335,8 +1335,8 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="21">
-        <f>[1]avgCover_ordered!$AA$28</f>
-        <v>77.7</v>
+        <f>[1]avgCover_ordered!$Z$28</f>
+        <v>91.2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
@@ -1344,32 +1344,32 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="19">
-        <f>[1]avgCover_ordered!$AA$27</f>
-        <v>88.3</v>
+        <f>[1]avgCover_ordered!$Z$27</f>
+        <v>94.7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="14">
-        <f>[1]avgCover_ordered!$AA$23</f>
-        <v>74.8</v>
+        <f>[1]avgCover_ordered!$Z$23</f>
+        <v>91.7</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
-        <f>[1]avgCover_ordered!$AA$25</f>
-        <v>88.1</v>
+        <f>[1]avgCover_ordered!$Z$25</f>
+        <v>92.4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="14">
-        <f>[1]avgCover_ordered!$AA$24</f>
-        <v>78.2</v>
+        <f>[1]avgCover_ordered!$Z$24</f>
+        <v>90.2</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="14">
-        <f>[1]avgCover_ordered!$AA$26</f>
-        <v>85</v>
+        <f>[1]avgCover_ordered!$Z$26</f>
+        <v>93.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>